<commit_message>
Rerunning Morfeusz + results
</commit_message>
<xml_diff>
--- a/data/results/Morfeusz_XPOS.xlsx
+++ b/data/results/Morfeusz_XPOS.xlsx
@@ -1346,7 +1346,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>brev:npun</t>
+          <t>brev:pun</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -6386,7 +6386,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>part</t>
+          <t>comp</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
@@ -12866,7 +12866,7 @@
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>ppron3:sg:loc:m1:ter:akc:npraep</t>
+          <t>ppron3:sg:gen:m1:ter:akc:npraep</t>
         </is>
       </c>
       <c r="E415" t="inlineStr">
@@ -23246,7 +23246,7 @@
       </c>
       <c r="D761" t="inlineStr">
         <is>
-          <t>praet:pl:n:imperf</t>
+          <t>praet:pl:f:imperf</t>
         </is>
       </c>
       <c r="E761" t="inlineStr">
@@ -34046,7 +34046,7 @@
       </c>
       <c r="D1121" t="inlineStr">
         <is>
-          <t>subst:sg:gen:n:ncol</t>
+          <t>adj:sg:gen:n:pos</t>
         </is>
       </c>
       <c r="E1121" t="inlineStr">
@@ -35606,7 +35606,7 @@
       </c>
       <c r="D1173" t="inlineStr">
         <is>
-          <t>inf:perf</t>
+          <t>inf:imperf</t>
         </is>
       </c>
       <c r="E1173" t="inlineStr">
@@ -36296,7 +36296,7 @@
       </c>
       <c r="D1196" t="inlineStr">
         <is>
-          <t>subst:sg:gen:f</t>
+          <t>subst:sg:acc:f</t>
         </is>
       </c>
       <c r="E1196" t="inlineStr">
@@ -55076,7 +55076,7 @@
       </c>
       <c r="D1822" t="inlineStr">
         <is>
-          <t>subst:sg:gen:f</t>
+          <t>adj:sg:gen:f:pos</t>
         </is>
       </c>
       <c r="E1822" t="inlineStr">
@@ -83486,7 +83486,7 @@
       </c>
       <c r="D2769" t="inlineStr">
         <is>
-          <t>subst:sg:loc:m3</t>
+          <t>subst:sg:loc:m1</t>
         </is>
       </c>
       <c r="E2769" t="inlineStr">

</xml_diff>